<commit_message>
exe de imprimir ticket
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint 8.xlsx
+++ b/Analisis/SPRINTs/Sprint 8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3582D56-ADCB-43FC-ABA0-D5030C1B140D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B3FD12-E1E4-4A9B-A98D-0DAC01451BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2742908B-3BCC-43B9-992A-47053D702CAA}"/>
   </bookViews>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F1DDF7-DA0F-45BB-A6BD-A06B1EB5C5CE}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60:C61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
actualizaciones del documento de word
1.	En compras enter despues de agregar compra.
2.	Las cajeras en el menu de ojito que vean primero el menu precio y despues el de ubicaciones.
3.	Corregir lo de impresion de tickets largos
4.	Que se impriman solo los tickets de complementos y devoluciones. El original ya no.
5.	Cambio en complementos no aparece
6.	En tickets agregar el total de piezas que llevan. faltan en complementos y devoluciones
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint 8.xlsx
+++ b/Analisis/SPRINTs/Sprint 8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D326BA8-5CF5-4BC1-94C7-D69084615FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B41B56-982D-4443-BFC7-C6099FC73375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2742908B-3BCC-43B9-992A-47053D702CAA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t xml:space="preserve">hipo eliminar producto del inventario </t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>erni</t>
+  </si>
+  <si>
+    <t>el enter en compras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consulta existencias </t>
+  </si>
+  <si>
+    <t>solo imprimir el ticket de la accion que se esta haciendo</t>
+  </si>
+  <si>
+    <t>Agregar municipio en clientes</t>
   </si>
 </sst>
 </file>
@@ -331,13 +343,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F1DDF7-DA0F-45BB-A6BD-A06B1EB5C5CE}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B68" sqref="B62:B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,16 +683,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -692,7 +704,7 @@
       <c r="F2" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -700,7 +712,7 @@
       <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -712,22 +724,22 @@
       <c r="F4" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>59</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L6" s="6"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>63</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -739,7 +751,7 @@
       <c r="F8" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -748,7 +760,7 @@
       <c r="F9" t="s">
         <v>65</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -757,19 +769,19 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -778,16 +790,16 @@
       <c r="C13" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L15" s="6"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -796,13 +808,13 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="6"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="6"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -811,19 +823,19 @@
       <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="L18" s="6"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="L19" s="6"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>45</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -832,13 +844,13 @@
       <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="6"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -847,25 +859,25 @@
       <c r="C23" t="s">
         <v>37</v>
       </c>
-      <c r="L23" s="6"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="L24" s="6"/>
+      <c r="L24" s="7"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="L25" s="6"/>
+      <c r="L25" s="7"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L26" s="6"/>
+      <c r="L26" s="7"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L27" s="6"/>
+      <c r="L27" s="7"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
@@ -875,7 +887,7 @@
       <c r="K29" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="6" t="s">
+      <c r="L29" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -886,7 +898,7 @@
       <c r="K30" t="s">
         <v>23</v>
       </c>
-      <c r="L30" s="6"/>
+      <c r="L30" s="7"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -895,7 +907,7 @@
       <c r="K31" t="s">
         <v>26</v>
       </c>
-      <c r="L31" s="6"/>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
@@ -904,7 +916,7 @@
       <c r="K32" t="s">
         <v>26</v>
       </c>
-      <c r="L32" s="6"/>
+      <c r="L32" s="7"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
@@ -913,7 +925,7 @@
       <c r="K33" t="s">
         <v>27</v>
       </c>
-      <c r="L33" s="6"/>
+      <c r="L33" s="7"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -922,7 +934,7 @@
       <c r="K34" t="s">
         <v>27</v>
       </c>
-      <c r="L34" s="6"/>
+      <c r="L34" s="7"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
@@ -943,13 +955,13 @@
       <c r="K35" t="s">
         <v>23</v>
       </c>
-      <c r="L35" s="6"/>
+      <c r="L35" s="7"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>6</v>
       </c>
-      <c r="L36" s="6"/>
+      <c r="L36" s="7"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
@@ -958,7 +970,7 @@
       <c r="E38" t="s">
         <v>32</v>
       </c>
-      <c r="L38" s="6" t="s">
+      <c r="L38" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -969,7 +981,7 @@
       <c r="E39" t="s">
         <v>33</v>
       </c>
-      <c r="L39" s="6"/>
+      <c r="L39" s="7"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M42" s="3" t="s">
@@ -1156,13 +1168,13 @@
       <c r="B56" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="5">
         <v>44362</v>
       </c>
-      <c r="G56" s="7">
+      <c r="G56" s="5">
         <v>44367</v>
       </c>
-      <c r="J56" s="7">
+      <c r="J56" s="5">
         <v>44392</v>
       </c>
       <c r="M56" t="s">
@@ -1249,6 +1261,26 @@
       </c>
       <c r="C64" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>